<commit_message>
new results in table1 and 2
</commit_message>
<xml_diff>
--- a/Results/20221006 sample5_subproblem_comparison.xlsx
+++ b/Results/20221006 sample5_subproblem_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA\OSU\Tornado_proposal\Git\Two_Stage_Robust_Tornado_Problem\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A88A63F-72AE-4532-9F32-DC8895E9C553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AB63D2-EC95-4C41-BCAC-D6E69EBD39C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="original_subproblem" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="28">
   <si>
     <t>Budget :</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Do_nothing</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -534,17 +537,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19D55DF-21E0-41A8-A0B2-8768F3EBD55F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32.7265625" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>30000000</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>3600.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>3600.22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -553,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>